<commit_message>
feat: schedule function added and email sender with all broke printers
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caua.paiva\repositorios\magna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968EDED0-E995-444F-8B1B-1081D5B0A69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABF2674-E3E2-48B3-9A76-3260A388CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>DIA</t>
   </si>
@@ -88,9 +88,6 @@
     <t>IP</t>
   </si>
   <si>
-    <t>Horário</t>
-  </si>
-  <si>
     <t>Impressora 1</t>
   </si>
   <si>
@@ -104,6 +101,18 @@
   </si>
   <si>
     <t>10.197.0.62</t>
+  </si>
+  <si>
+    <t>Impressora 4</t>
+  </si>
+  <si>
+    <t>10.197.0.11</t>
+  </si>
+  <si>
+    <t>Horario Inicial</t>
+  </si>
+  <si>
+    <t>Horario Final</t>
   </si>
 </sst>
 </file>
@@ -190,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -217,6 +226,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,13 +735,15 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -739,44 +754,73 @@
         <v>16</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="9">
-        <v>0.41666666666666669</v>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.375</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="C3" s="9">
-        <v>0.4375</v>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.38194444444444442</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="9">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.38888888888888901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9">
-        <v>0.45833333333333331</v>
+      <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.39583333333333298</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>

</xml_diff>

<commit_message>
feat: add time in table to email
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caua.paiva\repositorios\magna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABF2674-E3E2-48B3-9A76-3260A388CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A451FCB-7C36-41E8-806D-356238FF1746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquivo Testado" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>DIA</t>
   </si>
@@ -79,40 +79,70 @@
     <t>dia 10</t>
   </si>
   <si>
-    <t>10.197.0.60</t>
-  </si>
-  <si>
     <t>Nome da Impressora</t>
   </si>
   <si>
     <t>IP</t>
   </si>
   <si>
-    <t>Impressora 1</t>
-  </si>
-  <si>
-    <t>Impressora 2</t>
-  </si>
-  <si>
-    <t>10.197.0.61</t>
-  </si>
-  <si>
-    <t>Impressora 3</t>
-  </si>
-  <si>
-    <t>10.197.0.62</t>
-  </si>
-  <si>
-    <t>Impressora 4</t>
-  </si>
-  <si>
-    <t>10.197.0.11</t>
-  </si>
-  <si>
     <t>Horario Inicial</t>
   </si>
   <si>
     <t>Horario Final</t>
+  </si>
+  <si>
+    <t>10.197.1.33</t>
+  </si>
+  <si>
+    <t>10.197.1.34</t>
+  </si>
+  <si>
+    <t>10.197.1.35</t>
+  </si>
+  <si>
+    <t>10.197.1.36</t>
+  </si>
+  <si>
+    <t>10.197.1.47</t>
+  </si>
+  <si>
+    <t>10.197.1.39</t>
+  </si>
+  <si>
+    <t>10.197.1.45</t>
+  </si>
+  <si>
+    <t>10.197.1.44</t>
+  </si>
+  <si>
+    <t>10.197.1.46</t>
+  </si>
+  <si>
+    <t>Restaurante</t>
+  </si>
+  <si>
+    <t>Bar Praia</t>
+  </si>
+  <si>
+    <t>Bar Piscina</t>
+  </si>
+  <si>
+    <t>Bar Barco</t>
+  </si>
+  <si>
+    <t>Cozinha</t>
+  </si>
+  <si>
+    <t>Recepcao</t>
+  </si>
+  <si>
+    <t>Aparador Piscina</t>
+  </si>
+  <si>
+    <t>Tapiocaria</t>
+  </si>
+  <si>
+    <t>Adega</t>
   </si>
 </sst>
 </file>
@@ -170,10 +200,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -223,9 +250,6 @@
     </xf>
     <xf numFmtId="21" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -735,7 +759,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,104 +772,177 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0.375</v>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="9">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0.38194444444444442</v>
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.54166666666666696</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="9">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0.38888888888888901</v>
+        <v>0.46527777777777801</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.58333333333333304</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.47569444444444497</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C6" s="9">
+        <v>0.48611111111111099</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.66666666666666696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0.39583333333333298</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="C7" s="9">
+        <v>0.49652777777777801</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.70833333333333304</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F8" s="12"/>
+      <c r="A8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.50694444444444497</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.79166666666666696</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.52777777777777801</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.83333333333333304</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
finish aplication and modified some logs
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caua.paiva\repositorios\magna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A451FCB-7C36-41E8-806D-356238FF1746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557126B2-D3B4-42F4-8D0B-F353D371532B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="555" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquivo Testado" sheetId="1" r:id="rId1"/>
@@ -759,7 +759,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="D2" s="10">
-        <v>0.5</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>0.4548611111111111</v>
       </c>
       <c r="D3" s="10">
-        <v>0.54166666666666696</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
         <v>0.46527777777777801</v>
       </c>
       <c r="D4" s="10">
-        <v>0.58333333333333304</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>0.47569444444444497</v>
       </c>
       <c r="D5" s="10">
-        <v>0.625</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>0.48611111111111099</v>
       </c>
       <c r="D6" s="10">
-        <v>0.66666666666666696</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
         <v>0.49652777777777801</v>
       </c>
       <c r="D7" s="10">
-        <v>0.70833333333333304</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,7 +879,7 @@
         <v>0.50694444444444497</v>
       </c>
       <c r="D8" s="10">
-        <v>0.75</v>
+        <v>0.99998842592592596</v>
       </c>
       <c r="F8" s="11"/>
     </row>
@@ -894,7 +894,7 @@
         <v>0.51736111111111105</v>
       </c>
       <c r="D9" s="10">
-        <v>0.79166666666666696</v>
+        <v>0.99998842592592596</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -908,7 +908,7 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="D10" s="10">
-        <v>0.83333333333333304</v>
+        <v>0.99998842592592596</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>

</xml_diff>